<commit_message>
PCC QEDm 3.0.0 for Trial Implementation
</commit_message>
<xml_diff>
--- a/PCC/QEDm/StructureDefinition-IHE.QEDm.Query.Audit.Consumer.xlsx
+++ b/PCC/QEDm/StructureDefinition-IHE.QEDm.Query.Audit.Consumer.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>3.0.0-comment1</t>
+    <t>3.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-08-05T09:53:44-05:00</t>
+    <t>2024-12-05T12:45:27-06:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>